<commit_message>
Update docs with new fields - portal-ui #611, ingest-api #92
</commit_message>
<xml_diff>
--- a/docs/libraries/ingest-validation-tools/schemas/sample-block/sample-block.xlsx
+++ b/docs/libraries/ingest-validation-tools/schemas/sample-block/sample-block.xlsx
@@ -15,10 +15,10 @@
     <sheet name="volume_unit list" sheetId="6" r:id="rId6"/>
     <sheet name="pathology_distance_unit list" sheetId="7" r:id="rId7"/>
     <sheet name="preparation_media list" sheetId="8" r:id="rId8"/>
-    <sheet name="preparation_temperature list" sheetId="9" r:id="rId9"/>
+    <sheet name="preparation_condition list" sheetId="9" r:id="rId9"/>
     <sheet name="processing_time_unit list" sheetId="10" r:id="rId10"/>
     <sheet name="storage_media list" sheetId="11" r:id="rId11"/>
-    <sheet name="storage_temperature list" sheetId="12" r:id="rId12"/>
+    <sheet name="storage_method list" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -195,7 +195,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature for the preparation process.</t>
+          <t>The condition under which the preparation occurred, such as whether the sample was placed in dry ice during the preparation.</t>
         </r>
       </text>
     </comment>
@@ -247,7 +247,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature during storage, after preparation and before the assay is performed.</t>
+          <t>The method by which the sample was stored, after preparation and before the assay was performed.</t>
         </r>
       </text>
     </comment>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>version</t>
   </si>
@@ -414,31 +414,28 @@
     <t>None</t>
   </si>
   <si>
-    <t>preparation_temperature</t>
-  </si>
-  <si>
-    <t>Liquid Nitrogen</t>
-  </si>
-  <si>
-    <t>Liquid Nitrogen Vapor</t>
-  </si>
-  <si>
-    <t>Dry Ice</t>
-  </si>
-  <si>
-    <t>-80 Celsius</t>
-  </si>
-  <si>
-    <t>-20 Celsius</t>
-  </si>
-  <si>
-    <t>4 Celsius</t>
-  </si>
-  <si>
-    <t>24 Celsius (Room Temperature)</t>
-  </si>
-  <si>
-    <t>37 Celsius</t>
+    <t>preparation_condition</t>
+  </si>
+  <si>
+    <t>frozen in liquid nitrogen</t>
+  </si>
+  <si>
+    <t>frozen in liquid nitrogen vapor</t>
+  </si>
+  <si>
+    <t>frozen in ice</t>
+  </si>
+  <si>
+    <t>frozen in dry ice</t>
+  </si>
+  <si>
+    <t>frozen at -20 C</t>
+  </si>
+  <si>
+    <t>ambient temperature</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
   <si>
     <t>processing_time_value</t>
@@ -486,25 +483,19 @@
     <t>Carboxymethylcellulose (CMC)</t>
   </si>
   <si>
-    <t>storage_temperature</t>
-  </si>
-  <si>
-    <t>Liquid Nitrogen (Unspecified)</t>
-  </si>
-  <si>
-    <t>Liquid Nitrogen (Cryotube)</t>
-  </si>
-  <si>
-    <t>Liquid Nitrogen (Straw)</t>
-  </si>
-  <si>
-    <t>-80 Celsius (Unspecified)</t>
-  </si>
-  <si>
-    <t>-80 Celsius (Cryotube)</t>
-  </si>
-  <si>
-    <t>-80 Celsius (Straw)</t>
+    <t>storage_method</t>
+  </si>
+  <si>
+    <t>frozen at -80 C</t>
+  </si>
+  <si>
+    <t>refrigerator</t>
+  </si>
+  <si>
+    <t>incubated at 37 C</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
   <si>
     <t>quality_criteria</t>
@@ -912,25 +903,25 @@
         <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -972,8 +963,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_media list." sqref="L2:L1048576">
       <formula1>'preparation_media list'!$A$1:$A$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_temperature list." sqref="M2:M1048576">
-      <formula1>'preparation_temperature list'!$A$1:$A$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_condition list." sqref="M2:M1048576">
+      <formula1>'preparation_condition list'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="N2:N1048576">
       <formula1>-1e+307</formula1>
@@ -985,8 +976,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_media list." sqref="P2:P1048576">
       <formula1>'storage_media list'!$A$1:$A$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_temperature list." sqref="Q2:Q1048576">
-      <formula1>'storage_temperature list'!$A$1:$A$12</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_method list." sqref="Q2:Q1048576">
+      <formula1>'storage_method list'!$A$1:$A$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1052,22 +1043,22 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -1087,42 +1078,42 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -1137,7 +1128,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1145,62 +1136,57 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1422,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1477,11 +1463,6 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>